<commit_message>
added bar graph of percent change in CPI
</commit_message>
<xml_diff>
--- a/SCOPES DATA.xlsx
+++ b/SCOPES DATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RStudio\15-min-wage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AC4137-1CBC-4939-9B7F-D7F167B34747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9895AF15-FB73-487C-9C08-E7854BAD5D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{44DC6786-BD85-4ADE-8FB9-0D13823A1F19}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{44DC6786-BD85-4ADE-8FB9-0D13823A1F19}"/>
   </bookViews>
   <sheets>
     <sheet name="mastersheet" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="above15" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3465,10 +3466,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FC8B82-6C3D-42C8-ABD2-4922F3C604FD}">
   <dimension ref="A1:BV49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AU1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="BE7" sqref="BE7"/>
+      <selection pane="topRight" activeCell="BQ1" sqref="BQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19949,21 +19950,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100676A300B67BE7E4790F10446FEAAB5F2" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d1e7b3ea210cbd1bd95b4785bb4cdd01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="792b7a51-9e32-4ca2-a481-ab94957997a0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f32273e17264ec33ec5605dbd403039" ns3:_="">
     <xsd:import namespace="792b7a51-9e32-4ca2-a481-ab94957997a0"/>
@@ -20153,31 +20139,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197C2FD3-4F3B-4CF4-BC0B-5CC47CEA3F26}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="792b7a51-9e32-4ca2-a481-ab94957997a0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8583F70-7151-4AA5-B7B2-D044A2BC913D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33EBD07-5AC0-4DCE-A99A-553847885AE5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20193,4 +20170,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8583F70-7151-4AA5-B7B2-D044A2BC913D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197C2FD3-4F3B-4CF4-BC0B-5CC47CEA3F26}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="792b7a51-9e32-4ca2-a481-ab94957997a0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>